<commit_message>
cambios en arca 2 03.04.2025
</commit_message>
<xml_diff>
--- a/Horarios2025.xlsx
+++ b/Horarios2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00_ENGITHUB\Modulo02_JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5069D9-5B4B-4697-AC85-5C936885669B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EDC338-AA29-46F9-A2F9-5454AA47C499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB16EAB-46E4-4296-9FB2-5DEE8DAED3CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
   <si>
     <t>RECREO</t>
   </si>
@@ -58,13 +58,37 @@
   </si>
   <si>
     <t>SEGUNDO AÑO</t>
+  </si>
+  <si>
+    <t>LUNES</t>
+  </si>
+  <si>
+    <t>MARTES</t>
+  </si>
+  <si>
+    <t>MIERCOLES</t>
+  </si>
+  <si>
+    <t>JUEVES</t>
+  </si>
+  <si>
+    <t>VIERNES</t>
+  </si>
+  <si>
+    <t>TALLER 1</t>
+  </si>
+  <si>
+    <t>TALLER 2</t>
+  </si>
+  <si>
+    <t>NODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +107,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,13 +141,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF227ACB"/>
+        <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,26 +170,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,6 +209,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FF000000"/>
     </mruColors>
   </colors>
@@ -472,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB2B772-8170-4FFE-ABA1-AFA216428B0A}">
-  <dimension ref="B3:F35"/>
+  <dimension ref="B3:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,354 +534,597 @@
     <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="G3" s="8"/>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
         <v>0.625</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>0.63194444444444442</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>0.63888888888888884</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="D5" s="11"/>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
         <v>0.63888888888888884</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="D6" s="11"/>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
         <v>0.64583333333333304</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>0.65277777777777801</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="D7" s="11"/>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
         <v>0.65277777777777801</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>0.65972222222222199</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="D8" s="11"/>
+      <c r="J8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
         <v>0.65972222222222199</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>0.66666666666666696</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="D9" s="11"/>
+      <c r="J9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>0.67361111111111105</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="11"/>
+      <c r="F10" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="J10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
         <v>0.67361111111111105</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>0.68055555555555503</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="D11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="J11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <v>0.68055555555555503</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>0.6875</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="F12" s="12"/>
+      <c r="J12" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
         <v>0.6875</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>0.69444444444444398</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="F13" s="12"/>
+      <c r="J13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
         <v>0.69444444444444398</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>0.70138888888888895</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="D14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="J14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
         <v>0.70138888888888895</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="3">
         <v>0.70833333333333304</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+      <c r="D15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="J15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
         <v>0.70833333333333304</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>0.71527777777777701</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="D16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="J16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>0.71527777777777701</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>0.72222222222222199</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="D17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="J17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
         <v>0.72222222222222199</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>0.72916666666666596</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="F18" s="7" t="s">
+      <c r="D18" s="11"/>
+      <c r="F18" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+      <c r="J18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>0.72916666666666596</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>0.73611111111111005</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="11"/>
+      <c r="F19" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="J19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
         <v>0.73611111111111105</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="3">
         <v>0.74305555555555503</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
+      <c r="D20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="J20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>0.74305555555555503</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="3">
         <v>0.749999999999999</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
+      <c r="F21" s="12"/>
+      <c r="J21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>0.75</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="3">
         <v>0.75694444444444398</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
+      <c r="F22" s="12"/>
+      <c r="J22" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>0.75694444444444398</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="3">
         <v>0.76388888888888795</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
+      <c r="D23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="J23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>0.76388888888888795</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="3">
         <v>0.77083333333333204</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="D24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="J24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>0.77083333333333304</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>0.77777777777777701</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+      <c r="D25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="J25" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>0.77777777777777701</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="3">
         <v>0.78472222222222099</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="D26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="J26" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>0.78472222222222199</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="3">
         <v>0.79166666666666596</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="F27" s="7" t="s">
+      <c r="D27" s="11"/>
+      <c r="F27" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
         <v>0.79166666666666596</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>0.79861111111111005</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="F28" s="4" t="s">
+      <c r="D28" s="11"/>
+      <c r="F28" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="I28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
         <v>0.79861111111111005</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="3">
         <v>0.80555555555555403</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+      <c r="D29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="I29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
         <v>0.80555555555555558</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="3">
         <v>0.8125</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
+      <c r="D30" s="13"/>
+      <c r="F30" s="12"/>
+      <c r="I30" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
         <v>0.8125</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="3">
         <v>0.81944444444444442</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+      <c r="D31" s="13"/>
+      <c r="F31" s="12"/>
+      <c r="I31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
         <v>0.81944444444444442</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="3">
         <v>0.82638888888888884</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
+      <c r="D32" s="13"/>
+      <c r="F32" s="12"/>
+      <c r="I32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
         <v>0.82638888888888895</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="3">
         <v>0.83333333333333304</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="6">
+      <c r="D33" s="13"/>
+      <c r="F33" s="12"/>
+      <c r="I33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="3">
         <v>0.84027777777777801</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="6">
+      <c r="D34" s="13"/>
+      <c r="F34" s="12"/>
+      <c r="H34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
         <v>0.84027777777777801</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="3">
         <v>0.84722222222222199</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="F35" s="4"/>
+      <c r="D35" s="13"/>
+      <c r="F35" s="12"/>
+      <c r="H35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="15">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C36" s="15">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.86111111111111005</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>0.86111111111111105</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.86805555555555403</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
+        <v>0.86805555555555503</v>
+      </c>
+      <c r="C39" s="15">
+        <v>0.874999999999998</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
cambios en arca 04.08.2025
</commit_message>
<xml_diff>
--- a/Horarios2025.xlsx
+++ b/Horarios2025.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00_ENGITHUB\Modulo02_JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EDC338-AA29-46F9-A2F9-5454AA47C499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3176D3-5A23-4DC5-A51C-679910EADF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB16EAB-46E4-4296-9FB2-5DEE8DAED3CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4CB16EAB-46E4-4296-9FB2-5DEE8DAED3CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="TALLER1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="23">
   <si>
     <t>RECREO</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>NODO</t>
+  </si>
+  <si>
+    <t>PRIMER CUATRIMESTRE</t>
+  </si>
+  <si>
+    <t>SEGUNDO CUATRIMESTRE</t>
+  </si>
+  <si>
+    <t>VIERNES PROF. MALDONADO</t>
+  </si>
+  <si>
+    <t>HORA</t>
   </si>
 </sst>
 </file>
@@ -170,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -188,6 +200,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,10 +213,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB2B772-8170-4FFE-ABA1-AFA216428B0A}">
-  <dimension ref="B3:L42"/>
+  <dimension ref="B1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,9 +550,39 @@
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="H1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="N1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -564,110 +612,150 @@
       <c r="L3" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
         <v>0.625</v>
       </c>
       <c r="C4" s="3">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>0.63194444444444442</v>
       </c>
       <c r="C5" s="3">
         <v>0.63888888888888884</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="13"/>
       <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>0.63888888888888884</v>
       </c>
       <c r="C6" s="3">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="13"/>
       <c r="J6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>0.64583333333333304</v>
       </c>
       <c r="C7" s="3">
         <v>0.65277777777777801</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="13"/>
       <c r="J7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>0.65277777777777801</v>
       </c>
       <c r="C8" s="3">
         <v>0.65972222222222199</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="13"/>
       <c r="J8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>0.65972222222222199</v>
       </c>
       <c r="C9" s="3">
         <v>0.66666666666666696</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="13"/>
       <c r="J9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="V9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="X9" s="17"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>0.66666666666666696</v>
       </c>
       <c r="C10" s="3">
         <v>0.67361111111111105</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="F10" s="12" t="s">
+      <c r="D10" s="13"/>
+      <c r="F10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="S10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>0.67361111111111105</v>
       </c>
       <c r="C11" s="3">
         <v>0.68055555555555503</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="F11" s="14"/>
       <c r="J11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="S11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.67361111111111105</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>0.68055555555555503</v>
       </c>
@@ -677,101 +765,200 @@
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="14"/>
       <c r="J12" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="S12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0.68055555555555503</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>0.6875</v>
       </c>
       <c r="C13" s="3">
         <v>0.69444444444444398</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" s="14"/>
       <c r="J13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>0.69444444444444398</v>
       </c>
       <c r="C14" s="3">
         <v>0.70138888888888895</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="F14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0.69444444444444398</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>0.70138888888888895</v>
       </c>
       <c r="C15" s="3">
         <v>0.70833333333333304</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="14"/>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L15" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0.70138888888888895</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>0.70833333333333304</v>
       </c>
       <c r="C16" s="3">
         <v>0.71527777777777701</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="F16" s="14"/>
       <c r="J16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>0.71527777777777701</v>
       </c>
       <c r="C17" s="3">
         <v>0.72222222222222199</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="F17" s="14"/>
       <c r="J17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L17" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0.71527777777777701</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>0.72222222222222199</v>
       </c>
       <c r="C18" s="3">
         <v>0.72916666666666596</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="13"/>
       <c r="F18" s="2" t="s">
         <v>0</v>
       </c>
@@ -781,16 +968,28 @@
       <c r="L18" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>0.72916666666666596</v>
       </c>
       <c r="C19" s="3">
         <v>0.73611111111111005</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="F19" s="12" t="s">
+      <c r="D19" s="13"/>
+      <c r="F19" s="14" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="5" t="s">
@@ -799,24 +998,48 @@
       <c r="L19" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0.72916666666666596</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>0.73611111111111105</v>
       </c>
       <c r="C20" s="3">
         <v>0.74305555555555503</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="F20" s="14"/>
       <c r="J20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L20" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0.73611111111111005</v>
+      </c>
+      <c r="W20" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>0.74305555555555503</v>
       </c>
@@ -826,308 +1049,338 @@
       <c r="D21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="14"/>
       <c r="J21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="V21" s="3">
+        <v>0.74305555555555503</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>0.75</v>
       </c>
       <c r="C22" s="3">
         <v>0.75694444444444398</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="14"/>
       <c r="J22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>0.75694444444444398</v>
       </c>
       <c r="C23" s="3">
         <v>0.76388888888888795</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="F23" s="14"/>
       <c r="J23" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>0.76388888888888795</v>
       </c>
       <c r="C24" s="3">
         <v>0.77083333333333204</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="F24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="F24" s="14"/>
       <c r="J24" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>0.77083333333333304</v>
       </c>
       <c r="C25" s="3">
         <v>0.77777777777777701</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="F25" s="12"/>
+      <c r="D25" s="13"/>
+      <c r="F25" s="14"/>
       <c r="J25" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>0.77777777777777701</v>
       </c>
       <c r="C26" s="3">
         <v>0.78472222222222099</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="F26" s="12"/>
+      <c r="D26" s="13"/>
+      <c r="F26" s="14"/>
       <c r="J26" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>0.78472222222222199</v>
       </c>
       <c r="C27" s="3">
         <v>0.79166666666666596</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="13"/>
       <c r="F27" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>0.79166666666666596</v>
       </c>
       <c r="C28" s="3">
         <v>0.79861111111111005</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="F28" s="12" t="s">
+      <c r="D28" s="13"/>
+      <c r="F28" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>0.79861111111111005</v>
       </c>
       <c r="C29" s="3">
         <v>0.80555555555555403</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="F29" s="12"/>
-      <c r="I29" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="I29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>0.80555555555555558</v>
       </c>
       <c r="C30" s="3">
         <v>0.8125</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="F30" s="12"/>
-      <c r="I30" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D30" s="15"/>
+      <c r="F30" s="14"/>
+      <c r="I30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>0.8125</v>
       </c>
       <c r="C31" s="3">
         <v>0.81944444444444442</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="F31" s="12"/>
-      <c r="I31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="15"/>
+      <c r="F31" s="14"/>
+      <c r="I31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>0.81944444444444442</v>
       </c>
       <c r="C32" s="3">
         <v>0.82638888888888884</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="F32" s="12"/>
-      <c r="I32" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D32" s="15"/>
+      <c r="F32" s="14"/>
+      <c r="I32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>0.82638888888888895</v>
       </c>
       <c r="C33" s="3">
         <v>0.83333333333333304</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="F33" s="12"/>
-      <c r="I33" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="15"/>
+      <c r="F33" s="14"/>
+      <c r="I33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>0.83333333333333304</v>
       </c>
       <c r="C34" s="3">
         <v>0.84027777777777801</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="F34" s="12"/>
-      <c r="H34" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="15"/>
+      <c r="F34" s="14"/>
+      <c r="H34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>0.84027777777777801</v>
       </c>
       <c r="C35" s="3">
         <v>0.84722222222222199</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="F35" s="12"/>
-      <c r="H35" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
+      <c r="D35" s="15"/>
+      <c r="F35" s="14"/>
+      <c r="H35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="12">
         <v>0.84722222222222221</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="12">
         <v>0.85416666666666663</v>
       </c>
-      <c r="H36" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="15">
+      <c r="H36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="12">
         <v>0.85416666666666663</v>
       </c>
       <c r="C37" s="3">
         <v>0.86111111111111005</v>
       </c>
-      <c r="H37" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>0.86111111111111105</v>
       </c>
       <c r="C38" s="3">
         <v>0.86805555555555403</v>
       </c>
-      <c r="H38" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="15">
+      <c r="H38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
         <v>0.86805555555555503</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="12">
         <v>0.874999999999998</v>
       </c>
-      <c r="H39" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="15"/>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="12"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="H1:L2"/>
+    <mergeCell ref="N1:R2"/>
+    <mergeCell ref="W9:X9"/>
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="F19:F26"/>

</xml_diff>